<commit_message>
Addaing class in register form, student subject mapping in register form is implemented(all subject as initial student subject mapping)
</commit_message>
<xml_diff>
--- a/excelFiles/FORM_FOUR_REGISTRATION.xlsx
+++ b/excelFiles/FORM_FOUR_REGISTRATION.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>MTWARA ISLAMIC SECONDARY SCHOOL</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>0652445145</t>
+  </si>
+  <si>
+    <t>JUMA</t>
+  </si>
+  <si>
+    <t>HAMIDU</t>
+  </si>
+  <si>
+    <t>SALMA</t>
   </si>
 </sst>
 </file>
@@ -499,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,92 +754,168 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="F12" s="7"/>
-      <c r="H12" s="8"/>
+      <c r="A12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>31506</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>2001</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="F13" s="7"/>
-      <c r="H13" s="8"/>
+      <c r="A13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
+        <v>32967</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>2001</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
+      <c r="A14" s="9"/>
+      <c r="C14" s="9"/>
       <c r="F14" s="7"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
+      <c r="A15" s="9"/>
+      <c r="C15" s="9"/>
       <c r="F15" s="7"/>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
+      <c r="A16" s="9"/>
+      <c r="C16" s="9"/>
       <c r="F16" s="7"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
+      <c r="A17" s="9"/>
+      <c r="C17" s="9"/>
       <c r="F17" s="7"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="9"/>
+      <c r="C18" s="9"/>
       <c r="F18" s="7"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="9"/>
+      <c r="C19" s="9"/>
       <c r="F19" s="7"/>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+      <c r="A20" s="9"/>
+      <c r="C20" s="9"/>
       <c r="F20" s="7"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
+      <c r="A21" s="9"/>
+      <c r="C21" s="9"/>
       <c r="F21" s="7"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
+      <c r="A22" s="9"/>
+      <c r="C22" s="9"/>
       <c r="F22" s="7"/>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
+      <c r="A23" s="9"/>
+      <c r="C23" s="9"/>
       <c r="F23" s="7"/>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
+      <c r="A24" s="9"/>
+      <c r="C24" s="9"/>
       <c r="F24" s="7"/>
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
+      <c r="A25" s="9"/>
+      <c r="C25" s="9"/>
       <c r="F25" s="7"/>
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
+      <c r="A26" s="9"/>
+      <c r="C26" s="9"/>
       <c r="F26" s="7"/>
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
+      <c r="A27" s="9"/>
+      <c r="C27" s="9"/>
       <c r="F27" s="7"/>
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
+      <c r="A28" s="9"/>
+      <c r="C28" s="9"/>
       <c r="F28" s="7"/>
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
+      <c r="A29" s="9"/>
+      <c r="C29" s="9"/>
       <c r="F29" s="7"/>
       <c r="H29" s="8"/>
     </row>

</xml_diff>